<commit_message>
updates to group profile
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-patientlist.xlsx
+++ b/docs/StructureDefinition-patientlist.xlsx
@@ -4993,7 +4993,7 @@
         <v>39</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>38</v>
@@ -5098,7 +5098,7 @@
         <v>39</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>38</v>

</xml_diff>